<commit_message>
rangement Dashboard controller et CDCF
</commit_message>
<xml_diff>
--- a/EL_Electrical/CDCF SEISM.xlsx
+++ b/EL_Electrical/CDCF SEISM.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lecoc\Desktop\EPSA\Invictus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Romain\Documents\STUF-2020\EL_Electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2CF435C-B827-4761-83CD-29FE8AA24FC6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="4"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SEISM" sheetId="1" r:id="rId1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="180">
   <si>
     <t>Cahier des charges SEISM</t>
   </si>
@@ -298,9 +299,6 @@
     <t>FC2.1.5</t>
   </si>
   <si>
-    <t>a quantifier</t>
-  </si>
-  <si>
     <t>Visibilité</t>
   </si>
   <si>
@@ -551,12 +549,45 @@
   </si>
   <si>
     <t>Taux d'humidité</t>
+  </si>
+  <si>
+    <t>400g</t>
+  </si>
+  <si>
+    <t>surface</t>
+  </si>
+  <si>
+    <t>400mm²</t>
+  </si>
+  <si>
+    <t>environ 600mm² pour optimus</t>
+  </si>
+  <si>
+    <t>lisible en 0,2s</t>
+  </si>
+  <si>
+    <t>lisible en 0,4s</t>
+  </si>
+  <si>
+    <t>24mm de diamètre</t>
+  </si>
+  <si>
+    <t>accessible en 0,5s</t>
+  </si>
+  <si>
+    <t>feuille d'aluminium</t>
+  </si>
+  <si>
+    <t>tension de fonctionnement et protocoles</t>
+  </si>
+  <si>
+    <t>compatible CAN extended, fonctionnement sous 12v</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="#,##0\ &quot;€&quot;;[Red]\-#,##0\ &quot;€&quot;"/>
   </numFmts>
@@ -767,7 +798,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -916,6 +947,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -949,7 +983,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1335,56 +1369,56 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A2:E13" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
-  <autoFilter ref="A2:E13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A2:E13" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="A2:E13" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Fonctions principales" dataDxfId="25"/>
-    <tableColumn id="2" name="Fonctions contraintes" dataDxfId="24"/>
-    <tableColumn id="3" name="Critères " dataDxfId="23"/>
-    <tableColumn id="4" name="Niveau" dataDxfId="22"/>
-    <tableColumn id="5" name="Flexibilité" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Fonctions principales" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Fonctions contraintes" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Critères " dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Niveau" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Flexibilité" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau14" displayName="Tableau14" ref="A2:E19" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
-  <autoFilter ref="A2:E19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tableau14" displayName="Tableau14" ref="A2:E19" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+  <autoFilter ref="A2:E19" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Fonctions principales" dataDxfId="18"/>
-    <tableColumn id="2" name="Fonctions contraintes" dataDxfId="17"/>
-    <tableColumn id="3" name="Critères " dataDxfId="16"/>
-    <tableColumn id="4" name="Niveau" dataDxfId="15"/>
-    <tableColumn id="5" name="Flexibilité" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Fonctions principales" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Fonctions contraintes" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Critères " dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Niveau" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Flexibilité" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau16" displayName="Tableau16" ref="A2:E21" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A2:E21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tableau16" displayName="Tableau16" ref="A2:E21" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A2:E21" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Fonctions principales" dataDxfId="11"/>
-    <tableColumn id="2" name="Fonctions contraintes" dataDxfId="10"/>
-    <tableColumn id="3" name="Critères " dataDxfId="9"/>
-    <tableColumn id="4" name="Niveau" dataDxfId="8"/>
-    <tableColumn id="5" name="Flexibilité" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Fonctions principales" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Fonctions contraintes" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Critères " dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Niveau" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Flexibilité" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau15" displayName="Tableau15" ref="A2:E13" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A2:E13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tableau15" displayName="Tableau15" ref="A2:E13" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A2:E13" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Fonctions principales" dataDxfId="4"/>
-    <tableColumn id="2" name="Fonctions contraintes" dataDxfId="3"/>
-    <tableColumn id="3" name="Critères " dataDxfId="2"/>
-    <tableColumn id="4" name="Niveau" dataDxfId="1"/>
-    <tableColumn id="5" name="Flexibilité" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Fonctions principales" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Fonctions contraintes" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Critères " dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Niveau" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Flexibilité" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1652,41 +1686,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.77734375" style="1"/>
-    <col min="5" max="5" width="15.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.77734375" style="1"/>
+    <col min="1" max="1" width="31.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="1"/>
+    <col min="5" max="5" width="15.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="1"/>
     <col min="7" max="7" width="6" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.21875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" style="1" customWidth="1"/>
     <col min="9" max="9" width="10" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.77734375" style="1"/>
-    <col min="11" max="11" width="13.5546875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="13.33203125" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.77734375" style="1"/>
+    <col min="10" max="10" width="10.7109375" style="1"/>
+    <col min="11" max="11" width="13.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="50" t="s">
+    <row r="1" spans="1:6" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="52"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="53"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1704,7 +1738,7 @@
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>11</v>
       </c>
@@ -1722,7 +1756,7 @@
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="5" t="s">
         <v>13</v>
@@ -1731,14 +1765,14 @@
         <v>8</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E4" s="8">
         <v>0.2</v>
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7" t="s">
         <v>14</v>
@@ -1752,7 +1786,7 @@
       </c>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="7" t="s">
         <v>15</v>
@@ -1764,7 +1798,7 @@
       <c r="E6" s="7"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>16</v>
       </c>
@@ -1776,7 +1810,7 @@
       <c r="E7" s="7"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -1784,7 +1818,7 @@
       <c r="E8" s="7"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>17</v>
       </c>
@@ -1796,7 +1830,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -1804,7 +1838,7 @@
       <c r="E10" s="7"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
@@ -1816,7 +1850,7 @@
       <c r="E11" s="7"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -1824,19 +1858,19 @@
       <c r="E12" s="7"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="61" t="s">
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="50" t="s">
+        <v>113</v>
+      </c>
+      <c r="B13" s="43" t="s">
         <v>114</v>
-      </c>
-      <c r="B13" s="43" t="s">
-        <v>115</v>
       </c>
       <c r="C13" s="43"/>
       <c r="D13" s="43"/>
       <c r="E13" s="43"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="45"/>
       <c r="B14" s="45"/>
       <c r="C14" s="45"/>
@@ -1844,7 +1878,7 @@
       <c r="E14" s="45"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="45"/>
       <c r="B15" s="45"/>
       <c r="C15" s="45"/>
@@ -1852,7 +1886,7 @@
       <c r="E15" s="45"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="45"/>
       <c r="B16" s="45"/>
       <c r="C16" s="45"/>
@@ -1860,7 +1894,7 @@
       <c r="E16" s="45"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="45"/>
       <c r="B17" s="45"/>
       <c r="C17" s="45"/>
@@ -1868,7 +1902,7 @@
       <c r="E17" s="45"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="45"/>
       <c r="B18" s="45"/>
       <c r="C18" s="45"/>
@@ -1876,7 +1910,7 @@
       <c r="E18" s="45"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="45"/>
       <c r="B19" s="45"/>
       <c r="C19" s="45"/>
@@ -1884,7 +1918,7 @@
       <c r="E19" s="45"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="45"/>
       <c r="B20" s="45"/>
       <c r="C20" s="45"/>
@@ -1892,7 +1926,7 @@
       <c r="E20" s="45"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="45"/>
       <c r="B21" s="45"/>
       <c r="C21" s="45"/>
@@ -1900,7 +1934,7 @@
       <c r="E21" s="45"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="45"/>
       <c r="B22" s="45"/>
       <c r="C22" s="45"/>
@@ -1908,7 +1942,7 @@
       <c r="E22" s="45"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="45"/>
       <c r="B23" s="45"/>
       <c r="C23" s="45"/>
@@ -1916,7 +1950,7 @@
       <c r="E23" s="45"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="45"/>
       <c r="B24" s="45"/>
       <c r="C24" s="45"/>
@@ -1924,7 +1958,7 @@
       <c r="E24" s="45"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="45"/>
       <c r="B25" s="45"/>
       <c r="C25" s="45"/>
@@ -1932,7 +1966,7 @@
       <c r="E25" s="45"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="45"/>
       <c r="B26" s="45"/>
       <c r="C26" s="45"/>
@@ -1940,7 +1974,7 @@
       <c r="E26" s="45"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="45"/>
       <c r="B27" s="45"/>
       <c r="C27" s="45"/>
@@ -1948,7 +1982,7 @@
       <c r="E27" s="45"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="45"/>
       <c r="B28" s="45"/>
       <c r="C28" s="45"/>
@@ -1956,7 +1990,7 @@
       <c r="E28" s="45"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1977,33 +2011,33 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M204"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="27.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.21875" style="1" customWidth="1"/>
-    <col min="6" max="9" width="11.5546875" style="1"/>
-    <col min="10" max="12" width="11.6640625" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="1" width="28.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="1" customWidth="1"/>
+    <col min="6" max="9" width="11.5703125" style="1"/>
+    <col min="10" max="12" width="11.7109375" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="13" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="50" t="s">
+    <row r="1" spans="1:13" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="52"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="53"/>
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
       <c r="H1" s="11"/>
@@ -2013,7 +2047,7 @@
       <c r="L1" s="11"/>
       <c r="M1" s="12"/>
     </row>
-    <row r="2" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2038,7 +2072,7 @@
       <c r="L2" s="12"/>
       <c r="M2" s="12"/>
     </row>
-    <row r="3" spans="1:13" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>23</v>
       </c>
@@ -2055,7 +2089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="5" t="s">
         <v>13</v>
@@ -2070,7 +2104,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5" t="s">
         <v>14</v>
@@ -2085,7 +2119,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="5" t="s">
         <v>15</v>
@@ -2100,14 +2134,14 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:13" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>24</v>
       </c>
@@ -2124,25 +2158,25 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="13" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" s="13" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
       <c r="B9" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:13" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>28</v>
       </c>
@@ -2159,7 +2193,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5" t="s">
         <v>30</v>
@@ -2174,13 +2208,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>107</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>108</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>7</v>
@@ -2189,14 +2223,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:13" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>32</v>
       </c>
@@ -2204,7 +2238,7 @@
         <v>33</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D15" s="5">
         <v>0</v>
@@ -2213,46 +2247,46 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="1:5" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C17" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>111</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>112</v>
       </c>
       <c r="E17" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B19" s="39"/>
       <c r="C19" s="39" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D19" s="39" t="s">
         <v>7</v>
@@ -2261,251 +2295,251 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="41"/>
       <c r="B20" s="41"/>
       <c r="C20" s="41"/>
       <c r="D20" s="41"/>
       <c r="E20" s="41"/>
     </row>
-    <row r="21" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="41"/>
       <c r="B21" s="41"/>
       <c r="C21" s="41"/>
       <c r="D21" s="41"/>
       <c r="E21" s="41"/>
     </row>
-    <row r="22" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="41"/>
       <c r="B22" s="41"/>
       <c r="C22" s="41"/>
       <c r="D22" s="41"/>
       <c r="E22" s="41"/>
     </row>
-    <row r="23" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="41"/>
       <c r="B23" s="41"/>
       <c r="C23" s="41"/>
       <c r="D23" s="41"/>
       <c r="E23" s="41"/>
     </row>
-    <row r="24" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="41"/>
       <c r="B24" s="41"/>
       <c r="C24" s="41"/>
       <c r="D24" s="41"/>
       <c r="E24" s="41"/>
     </row>
-    <row r="25" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="41"/>
       <c r="B25" s="41"/>
       <c r="C25" s="41"/>
       <c r="D25" s="41"/>
       <c r="E25" s="41"/>
     </row>
-    <row r="26" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="41"/>
       <c r="B26" s="41"/>
       <c r="C26" s="41"/>
       <c r="D26" s="41"/>
       <c r="E26" s="41"/>
     </row>
-    <row r="27" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="41"/>
       <c r="B27" s="41"/>
       <c r="C27" s="41"/>
       <c r="D27" s="41"/>
       <c r="E27" s="41"/>
     </row>
-    <row r="28" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="41"/>
       <c r="B28" s="41"/>
       <c r="C28" s="41"/>
       <c r="D28" s="41"/>
       <c r="E28" s="41"/>
     </row>
-    <row r="29" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="41"/>
       <c r="B29" s="41"/>
       <c r="C29" s="41"/>
       <c r="D29" s="41"/>
       <c r="E29" s="41"/>
     </row>
-    <row r="30" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="33" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="34" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="35" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="36" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="37" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="38" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="39" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="40" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="41" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="42" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="43" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="44" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="45" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="46" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="47" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="48" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="49" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="50" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="51" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="52" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="53" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="54" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="55" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="56" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="57" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="58" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="59" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="60" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="61" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="62" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="63" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="64" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="65" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="66" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="67" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="68" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="69" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="70" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="71" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="72" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="73" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="74" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="75" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="76" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="77" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="78" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="79" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="80" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="81" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="82" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="83" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="84" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="85" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="86" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="87" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="88" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="89" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="90" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="91" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="92" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="93" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="94" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="95" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="96" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="97" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="98" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="99" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="100" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="101" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="102" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="103" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="104" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="105" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="106" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="107" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="108" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="109" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="110" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="111" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="112" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="113" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="114" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="115" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="116" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="117" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="118" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="119" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="120" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="121" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="122" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="123" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="124" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="125" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="126" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="127" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="128" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="129" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="130" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="131" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="132" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="133" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="134" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="135" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="136" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="137" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="138" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="139" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="140" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="141" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="142" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="143" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="144" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="145" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="146" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="147" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="148" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="149" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="150" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="151" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="152" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="153" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="154" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="155" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="156" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="157" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="158" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="159" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="160" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="161" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="162" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="163" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="164" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="165" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="166" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="167" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="168" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="169" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="170" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="171" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="172" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="173" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="174" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="175" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="176" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="177" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="178" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="179" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="180" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="181" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="182" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="183" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="184" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="185" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="186" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="187" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="188" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="189" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="190" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="191" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="192" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="193" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="194" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="195" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="196" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="197" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="198" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="199" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="200" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="201" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="202" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="203" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="204" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="95" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="96" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="97" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="98" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="99" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="100" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="101" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="102" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="103" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="104" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="105" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="106" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="107" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="108" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="109" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="110" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="111" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="112" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="113" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="114" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="115" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="116" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="117" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="118" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="119" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="120" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="121" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="122" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="123" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="124" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="125" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="126" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="127" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="128" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="129" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="130" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="131" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="132" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="133" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="134" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="135" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="136" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="137" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="138" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="139" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="140" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="141" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="142" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="143" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="144" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="145" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="146" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="147" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="148" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="149" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="150" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="151" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="152" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="153" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="154" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="155" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="156" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="157" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="158" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="159" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="160" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="161" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="162" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="163" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="164" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="165" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="166" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="167" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="168" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="169" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="170" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="171" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="172" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="173" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="174" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="175" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="176" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="177" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="178" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="179" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="180" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="181" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="182" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="183" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="184" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="185" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="186" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="187" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="188" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="189" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="190" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="191" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="192" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="193" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="194" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="195" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="196" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="197" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="198" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="199" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="200" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="201" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="202" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="203" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="204" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
@@ -2519,32 +2553,32 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.21875" customWidth="1"/>
-    <col min="2" max="2" width="24.77734375" customWidth="1"/>
+    <col min="1" max="1" width="33.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="50" t="s">
-        <v>134</v>
-      </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="52"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="51" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="53"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2561,7 +2595,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>23</v>
       </c>
@@ -2578,7 +2612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="5" t="s">
         <v>13</v>
@@ -2587,13 +2621,13 @@
         <v>8</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E4" s="8">
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7" t="s">
         <v>14</v>
@@ -2606,84 +2640,84 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>136</v>
-      </c>
       <c r="C8" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C9" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>163</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>164</v>
       </c>
       <c r="E9" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>139</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>140</v>
       </c>
       <c r="E11" s="8">
         <v>0.05</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="7" t="s">
@@ -2696,22 +2730,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>143</v>
-      </c>
       <c r="C15" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D15" s="7">
         <v>0</v>
@@ -2720,35 +2754,35 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="8">
         <v>0.05</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>146</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>147</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>7</v>
@@ -2757,105 +2791,105 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="8"/>
     </row>
-    <row r="20" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="C20" s="7" t="s">
         <v>149</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>150</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="43"/>
       <c r="B21" s="43" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C21" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D21" s="43" t="s">
         <v>167</v>
-      </c>
-      <c r="D21" s="43" t="s">
-        <v>168</v>
       </c>
       <c r="E21" s="44">
         <v>0.2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="45"/>
       <c r="B22" s="45"/>
       <c r="C22" s="45"/>
       <c r="D22" s="45"/>
       <c r="E22" s="45"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="45"/>
       <c r="B23" s="45"/>
       <c r="C23" s="45"/>
       <c r="D23" s="45"/>
       <c r="E23" s="45"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="45"/>
       <c r="B24" s="45"/>
       <c r="C24" s="45"/>
       <c r="D24" s="45"/>
       <c r="E24" s="45"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="45"/>
       <c r="B25" s="45"/>
       <c r="C25" s="45"/>
       <c r="D25" s="45"/>
       <c r="E25" s="45"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="45"/>
       <c r="B26" s="45"/>
       <c r="C26" s="45"/>
       <c r="D26" s="45"/>
       <c r="E26" s="45"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="45"/>
       <c r="B27" s="45"/>
       <c r="C27" s="45"/>
       <c r="D27" s="45"/>
       <c r="E27" s="45"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="45"/>
       <c r="B28" s="45"/>
       <c r="C28" s="45"/>
       <c r="D28" s="45"/>
       <c r="E28" s="45"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="45"/>
       <c r="B29" s="45"/>
       <c r="C29" s="45"/>
       <c r="D29" s="45"/>
       <c r="E29" s="45"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="45"/>
       <c r="B30" s="45"/>
       <c r="C30" s="45"/>
       <c r="D30" s="45"/>
       <c r="E30" s="45"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -2874,40 +2908,42 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="19" customWidth="1"/>
-    <col min="2" max="2" width="26.44140625" style="18" customWidth="1"/>
-    <col min="3" max="3" width="6.33203125" style="19" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" style="18" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" style="18" customWidth="1"/>
-    <col min="6" max="6" width="66.6640625" style="18" customWidth="1"/>
-    <col min="7" max="7" width="26.33203125" style="18" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" style="18" customWidth="1"/>
-    <col min="9" max="9" width="12.88671875" style="19" customWidth="1"/>
-    <col min="10" max="16384" width="11.44140625" style="18"/>
+    <col min="2" max="2" width="26.42578125" style="18" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" style="19" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="18" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="18" customWidth="1"/>
+    <col min="6" max="6" width="66.7109375" style="18" customWidth="1"/>
+    <col min="7" max="7" width="26.28515625" style="18" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" style="18" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" style="19" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="18"/>
+    <col min="11" max="11" width="36.140625" style="18" customWidth="1"/>
+    <col min="12" max="16384" width="11.42578125" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="22" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="53" t="s">
-        <v>102</v>
-      </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53" t="s">
+    <row r="1" spans="1:11" s="22" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="54" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
       <c r="G1" s="23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H1" s="23" t="s">
         <v>4</v>
@@ -2916,12 +2952,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="32"/>
@@ -2931,17 +2967,17 @@
       <c r="H2" s="25"/>
       <c r="I2" s="26"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
       <c r="B3" s="30"/>
       <c r="C3" s="31" t="s">
-        <v>154</v>
-      </c>
-      <c r="D3" s="56" t="s">
         <v>153</v>
       </c>
-      <c r="E3" s="57"/>
-      <c r="F3" s="58"/>
+      <c r="D3" s="57" t="s">
+        <v>152</v>
+      </c>
+      <c r="E3" s="58"/>
+      <c r="F3" s="59"/>
       <c r="G3" s="9" t="s">
         <v>6</v>
       </c>
@@ -2952,64 +2988,73 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="20"/>
       <c r="B4" s="30"/>
       <c r="C4" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="D4" s="59" t="s">
         <v>155</v>
       </c>
-      <c r="E4" s="59"/>
-      <c r="F4" s="60"/>
+      <c r="D4" s="60" t="s">
+        <v>154</v>
+      </c>
+      <c r="E4" s="60"/>
+      <c r="F4" s="61"/>
       <c r="G4" s="46" t="s">
         <v>8</v>
       </c>
       <c r="H4" s="46" t="s">
-        <v>37</v>
+        <v>169</v>
       </c>
       <c r="I4" s="47">
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="20"/>
       <c r="B5" s="30"/>
       <c r="C5" s="31" t="s">
-        <v>157</v>
-      </c>
-      <c r="D5" s="59" t="s">
-        <v>159</v>
-      </c>
-      <c r="E5" s="59"/>
-      <c r="F5" s="60"/>
+        <v>156</v>
+      </c>
+      <c r="D5" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="E5" s="60"/>
+      <c r="F5" s="61"/>
       <c r="G5" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="46"/>
+      <c r="H5" s="62">
+        <v>100</v>
+      </c>
       <c r="I5" s="47">
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20"/>
       <c r="B6" s="30"/>
       <c r="C6" s="31" t="s">
-        <v>158</v>
-      </c>
-      <c r="D6" s="59" t="s">
-        <v>160</v>
-      </c>
-      <c r="E6" s="59"/>
-      <c r="F6" s="60"/>
+        <v>157</v>
+      </c>
+      <c r="D6" s="60" t="s">
+        <v>159</v>
+      </c>
+      <c r="E6" s="60"/>
+      <c r="F6" s="61"/>
       <c r="G6" s="46" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="46"/>
-      <c r="I6" s="47"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v>170</v>
+      </c>
+      <c r="H6" s="46" t="s">
+        <v>171</v>
+      </c>
+      <c r="I6" s="47">
+        <v>0.1</v>
+      </c>
+      <c r="K6" s="18" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="20"/>
       <c r="B7" s="30"/>
       <c r="C7" s="31"/>
@@ -3020,101 +3065,101 @@
       <c r="H7" s="46"/>
       <c r="I7" s="47"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="54" t="s">
-        <v>98</v>
-      </c>
-      <c r="B8" s="55" t="s">
+    <row r="8" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="55" t="s">
         <v>97</v>
       </c>
+      <c r="B8" s="56" t="s">
+        <v>96</v>
+      </c>
       <c r="C8" s="36" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E8" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F8" s="33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G8" s="27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H8" s="27" t="s">
-        <v>85</v>
+        <v>173</v>
       </c>
       <c r="I8" s="29">
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="54"/>
-      <c r="B9" s="55"/>
+    <row r="9" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="55"/>
+      <c r="B9" s="56"/>
       <c r="C9" s="36"/>
       <c r="D9" s="33"/>
       <c r="E9" s="34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F9" s="33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G9" s="27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H9" s="27" t="s">
-        <v>85</v>
+        <v>174</v>
       </c>
       <c r="I9" s="29">
         <v>0.2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="54"/>
-      <c r="B10" s="55"/>
+    <row r="10" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="55"/>
+      <c r="B10" s="56"/>
       <c r="C10" s="36"/>
       <c r="D10" s="33"/>
       <c r="E10" s="34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F10" s="33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G10" s="27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H10" s="27" t="s">
-        <v>85</v>
+        <v>174</v>
       </c>
       <c r="I10" s="29">
         <v>0.2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="54"/>
-      <c r="B11" s="55"/>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="55"/>
+      <c r="B11" s="56"/>
       <c r="C11" s="36"/>
       <c r="D11" s="33"/>
       <c r="E11" s="34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F11" s="33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G11" s="27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H11" s="27" t="s">
-        <v>85</v>
+        <v>174</v>
       </c>
       <c r="I11" s="29">
         <v>0.2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="54"/>
-      <c r="B12" s="55"/>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="55"/>
+      <c r="B12" s="56"/>
       <c r="C12" s="36"/>
       <c r="D12" s="33"/>
       <c r="E12" s="34" t="s">
@@ -3127,15 +3172,15 @@
         <v>80</v>
       </c>
       <c r="H12" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="I12" s="29" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="54"/>
-      <c r="B13" s="55"/>
+        <v>173</v>
+      </c>
+      <c r="I12" s="29">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="55"/>
+      <c r="B13" s="56"/>
       <c r="C13" s="36"/>
       <c r="D13" s="33"/>
       <c r="E13" s="34" t="s">
@@ -3148,15 +3193,15 @@
         <v>80</v>
       </c>
       <c r="H13" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="I13" s="29" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="54"/>
-      <c r="B14" s="55"/>
+        <v>174</v>
+      </c>
+      <c r="I13" s="29">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="55"/>
+      <c r="B14" s="56"/>
       <c r="C14" s="36"/>
       <c r="D14" s="33"/>
       <c r="E14" s="34"/>
@@ -3165,9 +3210,9 @@
       <c r="H14" s="27"/>
       <c r="I14" s="29"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="54"/>
-      <c r="B15" s="55"/>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="55"/>
+      <c r="B15" s="56"/>
       <c r="C15" s="35" t="s">
         <v>79</v>
       </c>
@@ -3184,16 +3229,16 @@
         <v>6</v>
       </c>
       <c r="H15" s="25" t="s">
-        <v>7</v>
+        <v>175</v>
       </c>
       <c r="I15" s="26">
         <v>0</v>
       </c>
       <c r="J15" s="21"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="54"/>
-      <c r="B16" s="55"/>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="55"/>
+      <c r="B16" s="56"/>
       <c r="C16" s="35"/>
       <c r="D16" s="32"/>
       <c r="E16" s="31" t="s">
@@ -3212,9 +3257,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="54"/>
-      <c r="B17" s="55"/>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="55"/>
+      <c r="B17" s="56"/>
       <c r="C17" s="35"/>
       <c r="D17" s="32"/>
       <c r="E17" s="31" t="s">
@@ -3233,9 +3278,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="54"/>
-      <c r="B18" s="55"/>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="55"/>
+      <c r="B18" s="56"/>
       <c r="C18" s="35"/>
       <c r="D18" s="32"/>
       <c r="E18" s="31" t="s">
@@ -3251,12 +3296,12 @@
         <v>58</v>
       </c>
       <c r="I18" s="26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="54"/>
-      <c r="B19" s="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="55"/>
+      <c r="B19" s="56"/>
       <c r="C19" s="35"/>
       <c r="D19" s="32"/>
       <c r="E19" s="31" t="s">
@@ -3272,12 +3317,12 @@
         <v>58</v>
       </c>
       <c r="I19" s="26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="54"/>
-      <c r="B20" s="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="55"/>
+      <c r="B20" s="56"/>
       <c r="C20" s="31"/>
       <c r="D20" s="32"/>
       <c r="E20" s="31" t="s">
@@ -3293,12 +3338,12 @@
         <v>58</v>
       </c>
       <c r="I20" s="26">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="54"/>
-      <c r="B21" s="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="55"/>
+      <c r="B21" s="56"/>
       <c r="C21" s="31"/>
       <c r="D21" s="32"/>
       <c r="E21" s="31" t="s">
@@ -3314,12 +3359,12 @@
         <v>58</v>
       </c>
       <c r="I21" s="26">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="54"/>
-      <c r="B22" s="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="55"/>
+      <c r="B22" s="56"/>
       <c r="C22" s="31"/>
       <c r="D22" s="32"/>
       <c r="E22" s="31" t="s">
@@ -3335,12 +3380,12 @@
         <v>58</v>
       </c>
       <c r="I22" s="26">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="54"/>
-      <c r="B23" s="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="55"/>
+      <c r="B23" s="56"/>
       <c r="C23" s="31"/>
       <c r="D23" s="32"/>
       <c r="E23" s="31" t="s">
@@ -3356,10 +3401,10 @@
         <v>58</v>
       </c>
       <c r="I23" s="26">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="20"/>
       <c r="B24" s="37"/>
       <c r="C24" s="31"/>
@@ -3370,7 +3415,7 @@
       <c r="H24" s="25"/>
       <c r="I24" s="26"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>57</v>
       </c>
@@ -3388,10 +3433,14 @@
       <c r="G25" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="H25" s="27"/>
-      <c r="I25" s="28"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H25" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="I25" s="29">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="20"/>
       <c r="B26" s="30"/>
       <c r="C26" s="34"/>
@@ -3402,11 +3451,11 @@
       <c r="H26" s="27"/>
       <c r="I26" s="28"/>
     </row>
-    <row r="27" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="54" t="s">
+    <row r="27" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="55" t="s">
+      <c r="B27" s="56" t="s">
         <v>51</v>
       </c>
       <c r="C27" s="31" t="s">
@@ -3422,7 +3471,7 @@
         <v>41</v>
       </c>
       <c r="G27" s="25" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H27" s="25">
         <v>0</v>
@@ -3431,14 +3480,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="54"/>
-      <c r="B28" s="55"/>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="55"/>
+      <c r="B28" s="56"/>
       <c r="C28" s="31" t="s">
         <v>48</v>
       </c>
       <c r="D28" s="32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E28" s="35" t="s">
         <v>41</v>
@@ -3450,9 +3499,9 @@
       <c r="H28" s="25"/>
       <c r="I28" s="24"/>
     </row>
-    <row r="29" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="54"/>
-      <c r="B29" s="55"/>
+    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="55"/>
+      <c r="B29" s="56"/>
       <c r="C29" s="31" t="s">
         <v>47</v>
       </c>
@@ -3466,14 +3515,16 @@
         <v>41</v>
       </c>
       <c r="G29" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="H29" s="25"/>
+        <v>110</v>
+      </c>
+      <c r="H29" s="25" t="s">
+        <v>177</v>
+      </c>
       <c r="I29" s="26">
         <v>0.05</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="20"/>
       <c r="B30" s="37"/>
       <c r="C30" s="31"/>
@@ -3484,7 +3535,7 @@
       <c r="H30" s="25"/>
       <c r="I30" s="24"/>
     </row>
-    <row r="31" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>45</v>
       </c>
@@ -3503,9 +3554,15 @@
       <c r="F31" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="28"/>
+      <c r="G31" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="H31" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="I31" s="29">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -3526,31 +3583,31 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.44140625" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="50" t="s">
-        <v>132</v>
-      </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="52"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="51" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="53"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -3567,7 +3624,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>23</v>
       </c>
@@ -3584,7 +3641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="5" t="s">
         <v>13</v>
@@ -3599,7 +3656,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7" t="s">
         <v>14</v>
@@ -3614,7 +3671,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="7" t="s">
         <v>15</v>
@@ -3623,102 +3680,102 @@
         <v>10</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E6" s="8">
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>117</v>
-      </c>
       <c r="C8" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C9" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>126</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>127</v>
       </c>
       <c r="E9" s="8">
         <v>0.2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>123</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>124</v>
       </c>
       <c r="E10" s="8">
         <v>0.2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C12" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>129</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>130</v>
       </c>
       <c r="E12" s="8">
         <v>0.2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="50.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="43"/>
       <c r="B13" s="43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C13" s="43" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D13" s="43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E13" s="44">
         <v>0.2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="45"/>
       <c r="B14" s="45" t="s">
         <v>19</v>
@@ -3727,105 +3784,105 @@
       <c r="D14" s="45"/>
       <c r="E14" s="45"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="45"/>
       <c r="B15" s="45"/>
       <c r="C15" s="45"/>
       <c r="D15" s="45"/>
       <c r="E15" s="45"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="45"/>
       <c r="B16" s="45"/>
       <c r="C16" s="45"/>
       <c r="D16" s="45"/>
       <c r="E16" s="45"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="45"/>
       <c r="B17" s="45"/>
       <c r="C17" s="45"/>
       <c r="D17" s="45"/>
       <c r="E17" s="45"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="45"/>
       <c r="B18" s="45"/>
       <c r="C18" s="45"/>
       <c r="D18" s="45"/>
       <c r="E18" s="45"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="45"/>
       <c r="B19" s="45"/>
       <c r="C19" s="45"/>
       <c r="D19" s="45"/>
       <c r="E19" s="45"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="45"/>
       <c r="B20" s="45"/>
       <c r="C20" s="45"/>
       <c r="D20" s="45"/>
       <c r="E20" s="45"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="45"/>
       <c r="B21" s="45"/>
       <c r="C21" s="45"/>
       <c r="D21" s="45"/>
       <c r="E21" s="45"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="45"/>
       <c r="B22" s="45"/>
       <c r="C22" s="45"/>
       <c r="D22" s="45"/>
       <c r="E22" s="45"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="45"/>
       <c r="B23" s="45"/>
       <c r="C23" s="45"/>
       <c r="D23" s="45"/>
       <c r="E23" s="45"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="45"/>
       <c r="B24" s="45"/>
       <c r="C24" s="45"/>
       <c r="D24" s="45"/>
       <c r="E24" s="45"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="45"/>
       <c r="B25" s="45"/>
       <c r="C25" s="45"/>
       <c r="D25" s="45"/>
       <c r="E25" s="45"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="45"/>
       <c r="B26" s="45"/>
       <c r="C26" s="45"/>
       <c r="D26" s="45"/>
       <c r="E26" s="45"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="45"/>
       <c r="B27" s="45"/>
       <c r="C27" s="45"/>
       <c r="D27" s="45"/>
       <c r="E27" s="45"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="45"/>
       <c r="B28" s="45"/>
       <c r="C28" s="45"/>
       <c r="D28" s="45"/>
       <c r="E28" s="45"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="45"/>
       <c r="B29" s="45"/>
       <c r="C29" s="45"/>

</xml_diff>